<commit_message>
make passport ankera generation
</commit_message>
<xml_diff>
--- a/core/static/Анкерные_закладные/Расчет_анкерных_болтов.xlsx
+++ b/core/static/Анкерные_закладные/Расчет_анкерных_болтов.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE08886D-A582-4B13-AB7B-BD68D78F7D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C04C4C-FCB7-4150-98CB-C59A5DA7552C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Фланец" sheetId="4" r:id="rId1"/>
@@ -2322,16 +2322,16 @@
       </c>
       <c r="I19" s="15">
         <f ca="1">IF(H19=0,0,$E$22*SIN((H19-0.999)*2*PI()/$E$25))</f>
-        <v>9.9420596330613016E-5</v>
+        <v>1.491308935495056E-4</v>
       </c>
       <c r="J19" s="16">
         <f ca="1">I19*I19</f>
-        <v>9.8844549747347017E-9</v>
+        <v>2.2240023410873971E-8</v>
       </c>
       <c r="K19" s="17"/>
       <c r="L19" s="18">
         <f t="shared" ref="L19:L54" ca="1" si="0">$E$18*I19/$J$55</f>
-        <v>2.0311961391360052E-2</v>
+        <v>4.570191265683906E-2</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="AH19" s="88">
         <f ca="1">INT(AH17*AH3/SIN(360/2/E23*3.14159/180))+1</f>
-        <v>1653</v>
+        <v>1104</v>
       </c>
       <c r="AI19" s="86"/>
       <c r="AJ19" s="9" t="s">
@@ -2390,16 +2390,16 @@
       </c>
       <c r="I20" s="15">
         <f t="shared" ref="I20:I54" ca="1" si="2">IF(H20=0,0,$E$22*SIN((H20-1)*2*PI()/$E$25))</f>
-        <v>9.8916610967774904E-2</v>
+        <v>0.14743317862259717</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" ref="J20:J54" ca="1" si="3">I20*I20</f>
-        <v>9.7844959253501271E-3</v>
+        <v>2.1736542158762643E-2</v>
       </c>
       <c r="K20" s="17"/>
       <c r="L20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>20.208995490836418</v>
+        <v>45.181639375702815</v>
       </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
@@ -2447,16 +2447,16 @@
       </c>
       <c r="I21" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19482769076551429</v>
+        <v>0.28481902976691192</v>
       </c>
       <c r="J21" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7957829089022864E-2</v>
+        <v>8.1121879717365064E-2</v>
       </c>
       <c r="K21" s="17"/>
       <c r="L21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>39.803950879928919</v>
+        <v>87.284224694140889</v>
       </c>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
@@ -2503,16 +2503,16 @@
       </c>
       <c r="I22" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28481902976691192</v>
+        <v>0.40279493471831318</v>
       </c>
       <c r="J22" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1121879717365064E-2</v>
+        <v>0.16224375943473018</v>
       </c>
       <c r="K22" s="17"/>
       <c r="L22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>58.189483363305769</v>
+        <v>123.43853434367468</v>
       </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
@@ -2547,7 +2547,7 @@
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="54">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H23" s="49">
         <f t="shared" si="4"/>
@@ -2555,16 +2555,16 @@
       </c>
       <c r="I23" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36615628667422523</v>
+        <v>0.49332103051876397</v>
       </c>
       <c r="J23" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13407042627105742</v>
+        <v>0.24336563915209525</v>
       </c>
       <c r="K23" s="17"/>
       <c r="L23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>74.80695783998793</v>
+        <v>151.18071186951008</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -2614,16 +2614,16 @@
       </c>
       <c r="I24" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.43636807009496342</v>
+        <v>0.55022811334091037</v>
       </c>
       <c r="J24" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19041709259840292</v>
+        <v>0.30275097671069773</v>
       </c>
       <c r="K24" s="17"/>
       <c r="L24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>89.151460756849218</v>
+        <v>168.6201737193775</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -2666,7 +2666,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="50">
         <f>IF(E23=1,12,E23)</f>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H25" s="49">
         <f t="shared" si="4"/>
@@ -2674,16 +2674,16 @@
       </c>
       <c r="I25" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.49332103051876397</v>
+        <v>0.56963805953382396</v>
       </c>
       <c r="J25" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.24336563915209525</v>
+        <v>0.32448751886946037</v>
       </c>
       <c r="K25" s="17"/>
       <c r="L25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>100.78714165142952</v>
+        <v>174.56844938828181</v>
       </c>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="AH25" s="88">
         <f ca="1">AH19</f>
-        <v>1653</v>
+        <v>1104</v>
       </c>
       <c r="AI25" s="86" t="s">
         <v>89</v>
@@ -2731,16 +2731,16 @@
       </c>
       <c r="I26" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5352846810627383</v>
+        <v>0.55022811334091037</v>
       </c>
       <c r="J26" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28652968978043747</v>
+        <v>0.30275097671069773</v>
       </c>
       <c r="K26" s="17"/>
       <c r="L26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>109.36045624768563</v>
+        <v>168.6201737193775</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
@@ -2769,16 +2769,16 @@
       </c>
       <c r="I27" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5609839774397396</v>
+        <v>0.49332103051876403</v>
       </c>
       <c r="J27" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.31470302294411029</v>
+        <v>0.2433656391520953</v>
       </c>
       <c r="K27" s="17"/>
       <c r="L27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>114.61090871991686</v>
+        <v>151.18071186951011</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
@@ -2807,16 +2807,16 @@
       </c>
       <c r="I28" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.56963805953382396</v>
+        <v>0.40279493471831324</v>
       </c>
       <c r="J28" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.32448751886946037</v>
+        <v>0.16224375943473021</v>
       </c>
       <c r="K28" s="17"/>
       <c r="L28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>116.37896672661155</v>
+        <v>123.43853434367469</v>
       </c>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
@@ -2831,16 +2831,16 @@
       </c>
       <c r="I29" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5609839774397396</v>
+        <v>0.28481902976691192</v>
       </c>
       <c r="J29" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.31470302294411029</v>
+        <v>8.1121879717365064E-2</v>
       </c>
       <c r="K29" s="17"/>
       <c r="L29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>114.61090871991686</v>
+        <v>87.284224694140889</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
@@ -2855,16 +2855,16 @@
       </c>
       <c r="I30" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.53528468106273841</v>
+        <v>0.14743317862259733</v>
       </c>
       <c r="J30" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28652968978043758</v>
+        <v>2.1736542158762692E-2</v>
       </c>
       <c r="K30" s="17"/>
       <c r="L30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>109.36045624768565</v>
+        <v>45.181639375702865</v>
       </c>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
@@ -2879,16 +2879,16 @@
       </c>
       <c r="I31" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.49332103051876403</v>
+        <v>6.9789118849500894E-17</v>
       </c>
       <c r="J31" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2433656391520953</v>
+        <v>4.8705211097897609E-33</v>
       </c>
       <c r="K31" s="17"/>
       <c r="L31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>100.78714165142954</v>
+        <v>2.1387226604384708E-14</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
@@ -2900,16 +2900,16 @@
       </c>
       <c r="I32" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.43636807009496342</v>
+        <v>-0.14743317862259722</v>
       </c>
       <c r="J32" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19041709259840292</v>
+        <v>2.1736542158762657E-2</v>
       </c>
       <c r="K32" s="17"/>
       <c r="L32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>89.151460756849218</v>
+        <v>-45.181639375702829</v>
       </c>
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
@@ -2921,16 +2921,16 @@
       </c>
       <c r="I33" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.3661562866742254</v>
+        <v>-0.28481902976691181</v>
       </c>
       <c r="J33" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13407042627105753</v>
+        <v>8.1121879717364995E-2</v>
       </c>
       <c r="K33" s="17"/>
       <c r="L33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>74.806957839987959</v>
+        <v>-87.28422469414086</v>
       </c>
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
@@ -2942,16 +2942,16 @@
       </c>
       <c r="I34" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28481902976691215</v>
+        <v>-0.40279493471831296</v>
       </c>
       <c r="J34" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1121879717365189E-2</v>
+        <v>0.16224375943472999</v>
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>58.189483363305818</v>
+        <v>-123.4385343436746</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
@@ -2966,16 +2966,16 @@
       </c>
       <c r="I35" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19482769076551437</v>
+        <v>-0.49332103051876386</v>
       </c>
       <c r="J35" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7957829089022892E-2</v>
+        <v>0.24336563915209514</v>
       </c>
       <c r="K35" s="17"/>
       <c r="L35" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>39.803950879928934</v>
+        <v>-151.18071186951005</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -2990,16 +2990,16 @@
       </c>
       <c r="I36" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>9.8916610967774862E-2</v>
+        <v>-0.55022811334091037</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>9.7844959253501184E-3</v>
+        <v>0.30275097671069773</v>
       </c>
       <c r="K36" s="17"/>
       <c r="L36" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>20.208995490836408</v>
+        <v>-168.6201737193775</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -3013,16 +3013,16 @@
       </c>
       <c r="I37" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9789118849500894E-17</v>
+        <v>-0.56963805953382396</v>
       </c>
       <c r="J37" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8705211097897609E-33</v>
+        <v>0.32448751886946037</v>
       </c>
       <c r="K37" s="17"/>
       <c r="L37" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4258151126896985E-14</v>
+        <v>-174.56844938828181</v>
       </c>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="E38" s="25">
         <f ca="1">L55+E19/E23</f>
-        <v>118.75118894883377</v>
+        <v>178.12678272161514</v>
       </c>
       <c r="H38" s="49">
         <f t="shared" si="4"/>
@@ -3045,16 +3045,16 @@
       </c>
       <c r="I38" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-9.8916610967774724E-2</v>
+        <v>-0.55022811334091049</v>
       </c>
       <c r="J38" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>9.7844959253500906E-3</v>
+        <v>0.30275097671069784</v>
       </c>
       <c r="K38" s="17"/>
       <c r="L38" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.208995490836383</v>
+        <v>-168.62017371937753</v>
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="E39" s="29">
         <f ca="1">L55-E19/E23</f>
-        <v>114.00674450438933</v>
+        <v>171.01011605494847</v>
       </c>
       <c r="H39" s="49">
         <f t="shared" si="4"/>
@@ -3077,16 +3077,16 @@
       </c>
       <c r="I39" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.19482769076551423</v>
+        <v>-0.49332103051876397</v>
       </c>
       <c r="J39" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7957829089022843E-2</v>
+        <v>0.24336563915209525</v>
       </c>
       <c r="K39" s="17"/>
       <c r="L39" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-39.803950879928905</v>
+        <v>-151.18071186951008</v>
       </c>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
@@ -3098,16 +3098,16 @@
       </c>
       <c r="I40" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.28481902976691204</v>
+        <v>-0.40279493471831329</v>
       </c>
       <c r="J40" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>8.112187971736512E-2</v>
+        <v>0.16224375943473027</v>
       </c>
       <c r="K40" s="17"/>
       <c r="L40" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-58.18948336330579</v>
+        <v>-123.43853434367472</v>
       </c>
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
@@ -3140,22 +3140,22 @@
       </c>
       <c r="I41" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.36615628667422506</v>
+        <v>-0.28481902976691226</v>
       </c>
       <c r="J41" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13407042627105728</v>
+        <v>8.1121879717365244E-2</v>
       </c>
       <c r="K41" s="17"/>
       <c r="L41" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-74.806957839987902</v>
+        <v>-87.284224694140988</v>
       </c>
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="T41" s="79">
         <f ca="1">1.35*E38/W3*10</f>
-        <v>3.5625356684650136</v>
+        <v>5.3438034816484548</v>
       </c>
       <c r="U41" s="100">
         <f>INDEX(E43:E49,MATCH(F17,B43:B49,0))</f>
@@ -3176,16 +3176,16 @@
       </c>
       <c r="I42" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.43636807009496337</v>
+        <v>-0.14743317862259764</v>
       </c>
       <c r="J42" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19041709259840287</v>
+        <v>2.1736542158762782E-2</v>
       </c>
       <c r="K42" s="17"/>
       <c r="L42" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-89.151460756849218</v>
+        <v>-45.181639375702957</v>
       </c>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="D43" s="61">
         <f t="shared" ref="D43:D49" ca="1" si="5">$E$38/C43</f>
-        <v>0.74756807647991041</v>
+        <v>1.1213521103028967</v>
       </c>
       <c r="E43" s="34">
         <f>$W$3*T4/10</f>
@@ -3208,24 +3208,24 @@
       </c>
       <c r="F43" s="63">
         <f ca="1">$E$39/E43</f>
-        <v>0.71770062640471721</v>
+        <v>1.0765509351901068</v>
       </c>
       <c r="H43" s="49">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I43" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.49332103051876386</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J43" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.24336563915209514</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K43" s="17"/>
       <c r="L43" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-100.78714165142949</v>
+        <v>0</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="D44" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.47030173841122286</v>
+        <v>0.70545260483807981</v>
       </c>
       <c r="E44" s="34">
         <f>$W$3*T5/10</f>
@@ -3247,24 +3247,24 @@
       </c>
       <c r="F44" s="63">
         <f t="shared" ref="F44:F49" ca="1" si="6">$E$39/E44</f>
-        <v>0.45160128542043704</v>
+        <v>0.67740192535135069</v>
       </c>
       <c r="H44" s="49">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I44" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.53528468106273841</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J44" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.28652968978043758</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K44" s="17"/>
       <c r="L44" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-109.36045624768565</v>
+        <v>0</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
@@ -3278,7 +3278,7 @@
       </c>
       <c r="D45" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.32339648406545146</v>
+        <v>0.48509472418740507</v>
       </c>
       <c r="E45" s="34">
         <f t="shared" ref="E45:E49" si="7">$W$3*T6/10</f>
@@ -3286,24 +3286,24 @@
       </c>
       <c r="F45" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.31047588372655049</v>
+        <v>0.46571382367905356</v>
       </c>
       <c r="H45" s="49">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="I45" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.5609839774397396</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J45" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.31470302294411029</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K45" s="17"/>
       <c r="L45" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-114.61090871991686</v>
+        <v>0</v>
       </c>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="D46" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.23561743839054319</v>
+        <v>0.35342615619368084</v>
       </c>
       <c r="E46" s="34">
         <f t="shared" si="7"/>
@@ -3325,24 +3325,24 @@
       </c>
       <c r="F46" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.22620385814362962</v>
+        <v>0.33930578582331045</v>
       </c>
       <c r="H46" s="49">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I46" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.56963805953382396</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J46" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.32448751886946037</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K46" s="17"/>
       <c r="L46" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-116.37896672661155</v>
+        <v>0</v>
       </c>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="D47" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.17927413790584809</v>
+        <v>0.26891120579953975</v>
       </c>
       <c r="E47" s="34">
         <f t="shared" si="7"/>
@@ -3365,24 +3365,24 @@
       </c>
       <c r="F47" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.17211163119623993</v>
+        <v>0.25816744573512751</v>
       </c>
       <c r="H47" s="49">
         <f t="shared" si="4"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="I47" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.5609839774397396</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J47" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.31470302294411029</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K47" s="17"/>
       <c r="L47" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-114.61090871991686</v>
+        <v>0</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="D48" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.15010894823515836</v>
+        <v>0.22516342146582627</v>
       </c>
       <c r="E48" s="34">
         <f t="shared" si="7"/>
@@ -3405,24 +3405,24 @@
       </c>
       <c r="F48" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.14411167299252856</v>
+        <v>0.21616750860188155</v>
       </c>
       <c r="H48" s="49">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I48" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.5352846810627383</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J48" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.28652968978043747</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K48" s="17"/>
       <c r="L48" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-109.36045624768563</v>
+        <v>0</v>
       </c>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="D49" s="62">
         <f t="shared" ca="1" si="5"/>
-        <v>0.12999582807754106</v>
+        <v>0.19499374134823771</v>
       </c>
       <c r="E49" s="34">
         <f t="shared" si="7"/>
@@ -3445,24 +3445,24 @@
       </c>
       <c r="F49" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.12480212863096807</v>
+        <v>0.18720319217837819</v>
       </c>
       <c r="H49" s="49">
         <f t="shared" si="4"/>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I49" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.49332103051876419</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J49" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.24336563915209547</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K49" s="17"/>
       <c r="L49" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-100.78714165142958</v>
+        <v>0</v>
       </c>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
@@ -3470,20 +3470,20 @@
     <row r="50" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H50" s="49">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I50" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.43636807009496348</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J50" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.19041709259840295</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K50" s="17"/>
       <c r="L50" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-89.151460756849232</v>
+        <v>0</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
@@ -3499,20 +3499,20 @@
       <c r="F51" s="103"/>
       <c r="H51" s="49">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="I51" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.36615628667422545</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J51" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.13407042627105756</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K51" s="17"/>
       <c r="L51" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-74.806957839987973</v>
+        <v>0</v>
       </c>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
@@ -3520,20 +3520,20 @@
     <row r="52" spans="2:14" x14ac:dyDescent="0.3">
       <c r="H52" s="49">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="I52" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.28481902976691181</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J52" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>8.1121879717364995E-2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K52" s="17"/>
       <c r="L52" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-58.189483363305747</v>
+        <v>0</v>
       </c>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
@@ -3541,20 +3541,20 @@
     <row r="53" spans="2:14" x14ac:dyDescent="0.3">
       <c r="H53" s="49">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I53" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.19482769076551421</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J53" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.7957829089022829E-2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K53" s="17"/>
       <c r="L53" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-39.803950879928898</v>
+        <v>0</v>
       </c>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
@@ -3562,20 +3562,20 @@
     <row r="54" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H54" s="49">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I54" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-9.8916610967774932E-2</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J54" s="16">
-        <f t="shared" ca="1" si="3"/>
-        <v>9.7844959253501323E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K54" s="37"/>
       <c r="L54" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.208995490836422</v>
+        <v>0</v>
       </c>
       <c r="M54" s="37"/>
       <c r="N54" s="37"/>
@@ -3590,17 +3590,17 @@
       </c>
       <c r="H55" s="38">
         <f>MAX(H19:H54)</f>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="I55" s="28"/>
       <c r="J55" s="39">
         <f ca="1">SUM(J19:J54)</f>
-        <v>5.8407753495347423</v>
+        <v>3.893850248673548</v>
       </c>
       <c r="K55" s="28"/>
       <c r="L55" s="40">
         <f ca="1">MAX(L19:L54)</f>
-        <v>116.37896672661155</v>
+        <v>174.56844938828181</v>
       </c>
       <c r="M55" s="40">
         <f>SUM(M19:M54)</f>

</xml_diff>